<commit_message>
Limite de Credito E3 - Finalizado
</commit_message>
<xml_diff>
--- a/Data/TempExcelExport/Clientes con incidencias LC.xlsx
+++ b/Data/TempExcelExport/Clientes con incidencias LC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup.sharepoint.com/sites/IBERICAN_FCI/Shared Documents/1. Clientes/2. Límites de Crédito/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="8_{7AC7CC33-7575-48E7-9E50-6B79B30A2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21D69E0E-B33F-424B-B7E0-1F77D1350B60}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{7AC7CC33-7575-48E7-9E50-6B79B30A2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D40AA2DB-E24B-49F4-AF65-936ABAE11822}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{80C2A359-1417-4DB8-9FCF-050718A4EF94}"/>
+    <workbookView xWindow="13665" yWindow="345" windowWidth="18705" windowHeight="13815" xr2:uid="{80C2A359-1417-4DB8-9FCF-050718A4EF94}"/>
   </bookViews>
   <sheets>
     <sheet name="ES" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
   <si>
     <t>Cliente</t>
   </si>
@@ -263,13 +263,22 @@
   </si>
   <si>
     <t>Live Our Style</t>
+  </si>
+  <si>
+    <t>24050970  </t>
+  </si>
+  <si>
+    <t>Antonio Fernandez Del Riego</t>
+  </si>
+  <si>
+    <t>NO LIBERAR NADA,VZ7 solicita precaución</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,7 +408,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,9 +425,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -456,7 +465,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -562,7 +571,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -704,7 +713,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -713,13 +722,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC2B6E0-CB86-444E-845A-38B69EC4F7CA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.75" style="3" bestFit="1" customWidth="1"/>
@@ -728,7 +737,7 @@
     <col min="5" max="16384" width="8.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25" thickTop="1" thickBot="1">
+    <row r="1" spans="1:4" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -742,7 +751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.25" thickTop="1" thickBot="1">
+    <row r="2" spans="1:4" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>24370950</v>
       </c>
@@ -756,7 +765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" thickBot="1">
+    <row r="3" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>24460900</v>
       </c>
@@ -770,7 +779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" thickBot="1">
+    <row r="4" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>24291920</v>
       </c>
@@ -784,7 +793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.5" thickBot="1">
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>24040720</v>
       </c>
@@ -798,7 +807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13.5" thickBot="1">
+    <row r="6" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>24440820</v>
       </c>
@@ -812,7 +821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13.5" thickBot="1">
+    <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>24330260</v>
       </c>
@@ -826,7 +835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="13.5" thickBot="1">
+    <row r="8" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>24370920</v>
       </c>
@@ -840,7 +849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="13.5" thickBot="1">
+    <row r="9" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>24150930</v>
       </c>
@@ -854,7 +863,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" thickBot="1">
+    <row r="10" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>24310810</v>
       </c>
@@ -868,7 +877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" thickBot="1">
+    <row r="11" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>24360040</v>
       </c>
@@ -882,7 +891,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.5" thickBot="1">
+    <row r="12" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>24160920</v>
       </c>
@@ -896,7 +905,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="13.5" thickBot="1">
+    <row r="13" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>24410190</v>
       </c>
@@ -910,7 +919,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="13.5" thickBot="1">
+    <row r="14" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>24040650</v>
       </c>
@@ -924,7 +933,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="13.5" thickBot="1">
+    <row r="15" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>24356000</v>
       </c>
@@ -938,7 +947,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13.5" thickBot="1">
+    <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
@@ -952,7 +961,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13.5" thickBot="1">
+    <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>24100070</v>
       </c>
@@ -966,7 +975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="13.5" thickBot="1">
+    <row r="18" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>24062760</v>
       </c>
@@ -980,7 +989,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="13.5" thickBot="1">
+    <row r="19" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>24320360</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="13.5" thickBot="1">
+    <row r="20" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>24460620</v>
       </c>
@@ -1008,7 +1017,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="13.5" thickBot="1">
+    <row r="21" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>24160540</v>
       </c>
@@ -1022,7 +1031,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="13.5" thickBot="1">
+    <row r="22" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>24160870</v>
       </c>
@@ -1036,7 +1045,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="13.5" thickBot="1">
+    <row r="23" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>24450220</v>
       </c>
@@ -1050,7 +1059,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="13.5" thickBot="1">
+    <row r="24" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>24140420</v>
       </c>
@@ -1064,7 +1073,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="13.5" thickBot="1">
+    <row r="25" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24380400</v>
       </c>
@@ -1078,7 +1087,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="13.5" thickBot="1">
+    <row r="26" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24350380</v>
       </c>
@@ -1092,7 +1101,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="13.5" thickBot="1">
+    <row r="27" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>24380330</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="13.5" thickBot="1">
+    <row r="28" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>24050950</v>
       </c>
@@ -1120,7 +1129,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="13.5" thickBot="1">
+    <row r="29" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>24410480</v>
       </c>
@@ -1134,7 +1143,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="13.5" thickBot="1">
+    <row r="30" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>24292010</v>
       </c>
@@ -1148,7 +1157,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13.5" thickBot="1">
+    <row r="31" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>24292010</v>
       </c>
@@ -1160,6 +1169,20 @@
       </c>
       <c r="D31" s="3" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1174,7 +1197,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:C3 B4:B31</xm:sqref>
+          <xm:sqref>B2:C3 B4:B32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1191,17 +1214,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:1" ht="15" thickTop="1">
+    <row r="2" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1223,7 +1246,7 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
@@ -1231,7 +1254,7 @@
     <col min="4" max="4" width="39.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1">
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>46710570</v>
       </c>
@@ -1259,7 +1282,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>46730050</v>
       </c>
@@ -1273,7 +1296,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>46680120</v>
       </c>
@@ -1287,7 +1310,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>46700030</v>
       </c>
@@ -1301,7 +1324,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>46730280</v>
       </c>
@@ -1315,7 +1338,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>46750090</v>
       </c>
@@ -1329,7 +1352,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>46730070</v>
       </c>
@@ -1343,7 +1366,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>46730250</v>
       </c>
@@ -1357,7 +1380,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>46730290</v>
       </c>
@@ -1371,7 +1394,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>46680190</v>
       </c>
@@ -1385,7 +1408,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>46730180</v>
       </c>
@@ -1399,7 +1422,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>46710600</v>
       </c>
@@ -1413,7 +1436,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>46750050</v>
       </c>
@@ -1427,7 +1450,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>73</v>
       </c>
@@ -1441,91 +1464,91 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1552,26 +1575,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100812FB67C5E01F547A18D4A5FD6A8713D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b9642c6788bad27e02d635fb107c9ae4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xmlns:ns3="d9b07192-7579-4291-b28e-58bbe42d995f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e8472eb4e8570153d151932821fc84c" ns2:_="" ns3:_="">
     <xsd:import namespace="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
@@ -1806,14 +1809,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498E4CA6-DBB7-44FA-89D6-924D2B3C9ABD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DFC932F-8B19-4888-9E6D-5ED99EBC92C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
+    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85648A9D-E349-4AED-A783-3910A6F0B756}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85648A9D-E349-4AED-A783-3910A6F0B756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DFC932F-8B19-4888-9E6D-5ED99EBC92C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498E4CA6-DBB7-44FA-89D6-924D2B3C9ABD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
+    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Proceso finalizado en PRD
</commit_message>
<xml_diff>
--- a/Data/TempExcelExport/Clientes con incidencias LC.xlsx
+++ b/Data/TempExcelExport/Clientes con incidencias LC.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup.sharepoint.com/sites/IBERICAN_FCI/Shared Documents/1. Clientes/2. Límites de Crédito/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="8_{7AC7CC33-7575-48E7-9E50-6B79B30A2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D40AA2DB-E24B-49F4-AF65-936ABAE11822}"/>
+  <xr:revisionPtr revIDLastSave="249" documentId="8_{7AC7CC33-7575-48E7-9E50-6B79B30A2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E255FB40-95EF-4DCB-A8A7-A71C9E7A6349}"/>
   <bookViews>
-    <workbookView xWindow="13665" yWindow="345" windowWidth="18705" windowHeight="13815" xr2:uid="{80C2A359-1417-4DB8-9FCF-050718A4EF94}"/>
+    <workbookView xWindow="14460" yWindow="135" windowWidth="14340" windowHeight="15195" firstSheet="1" activeTab="1" xr2:uid="{80C2A359-1417-4DB8-9FCF-050718A4EF94}"/>
   </bookViews>
   <sheets>
-    <sheet name="ES" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" state="veryHidden" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" state="veryHidden" r:id="rId1"/>
+    <sheet name="ES" sheetId="1" r:id="rId2"/>
     <sheet name="PT" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
   <si>
     <t>Cliente</t>
   </si>
@@ -199,9 +199,6 @@
     <t>Joaquin Hernandez E Hijos, S.L</t>
   </si>
   <si>
-    <t>Davide Manuel</t>
-  </si>
-  <si>
     <t>Felijardim de Mario Felicia</t>
   </si>
   <si>
@@ -272,13 +269,28 @@
   </si>
   <si>
     <t>NO LIBERAR NADA,VZ7 solicita precaución</t>
+  </si>
+  <si>
+    <t>Alba Fernandez Fernandez / 39691 Iruz</t>
+  </si>
+  <si>
+    <t>Agroavícola Nalón</t>
+  </si>
+  <si>
+    <t>Ibarra Totana, S.L.</t>
+  </si>
+  <si>
+    <t>No liberar, tiene impagado</t>
+  </si>
+  <si>
+    <t>Davide Manuel Alves Da Silva</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +351,10 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -390,9 +406,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -407,9 +424,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{7AE600F6-D9FB-438A-A863-7ECA61E526E3}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -720,12 +738,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9297A7B3-2BBA-457A-A379-E12B8E985020}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial"&amp;10&amp;K000000 Intern | Internal&amp;1#_x000D_</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC2B6E0-CB86-444E-845A-38B69EC4F7CA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -994,7 +1044,7 @@
         <v>24320360</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>36</v>
@@ -1148,7 +1198,7 @@
         <v>24292010</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>52</v>
@@ -1158,31 +1208,70 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
-        <v>24292010</v>
+      <c r="A31" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>75</v>
+      <c r="A32" s="5">
+        <v>24062820</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="3" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>24050540</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>24380290</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>24160890</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1197,43 +1286,11 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:C3 B4:B32</xm:sqref>
+          <xm:sqref>B2:C3 B4:B35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9297A7B3-2BBA-457A-A379-E12B8E985020}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial"&amp;10&amp;K000000 Intern | Internal&amp;1#_x000D_</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -1276,10 +1333,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1290,10 +1347,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1304,10 +1361,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1318,10 +1375,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1332,10 +1389,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1346,10 +1403,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1360,10 +1417,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1374,10 +1431,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1388,10 +1445,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1402,10 +1459,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1416,10 +1473,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1430,10 +1487,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1444,24 +1501,24 @@
         <v>4</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1575,6 +1632,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100812FB67C5E01F547A18D4A5FD6A8713D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b9642c6788bad27e02d635fb107c9ae4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xmlns:ns3="d9b07192-7579-4291-b28e-58bbe42d995f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e8472eb4e8570153d151932821fc84c" ns2:_="" ns3:_="">
     <xsd:import namespace="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
@@ -1809,27 +1886,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85648A9D-E349-4AED-A783-3910A6F0B756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498E4CA6-DBB7-44FA-89D6-924D2B3C9ABD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
+    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DFC932F-8B19-4888-9E6D-5ED99EBC92C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1846,23 +1922,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85648A9D-E349-4AED-A783-3910A6F0B756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498E4CA6-DBB7-44FA-89D6-924D2B3C9ABD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
-    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Versión 1.0.43 PRD - Actualización GIT
</commit_message>
<xml_diff>
--- a/Data/TempExcelExport/Clientes con incidencias LC.xlsx
+++ b/Data/TempExcelExport/Clientes con incidencias LC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup.sharepoint.com/sites/IBERICAN_FCI/Shared Documents/1. Clientes/2. Límites de Crédito/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="249" documentId="8_{7AC7CC33-7575-48E7-9E50-6B79B30A2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E255FB40-95EF-4DCB-A8A7-A71C9E7A6349}"/>
+  <xr:revisionPtr revIDLastSave="324" documentId="8_{7AC7CC33-7575-48E7-9E50-6B79B30A2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAC99C16-B388-434A-AF5D-2B375FB0E8E9}"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="135" windowWidth="14340" windowHeight="15195" firstSheet="1" activeTab="1" xr2:uid="{80C2A359-1417-4DB8-9FCF-050718A4EF94}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="13125" windowHeight="11235" firstSheet="1" activeTab="1" xr2:uid="{80C2A359-1417-4DB8-9FCF-050718A4EF94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" state="veryHidden" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="97">
   <si>
     <t>Cliente</t>
   </si>
@@ -284,13 +284,58 @@
   </si>
   <si>
     <t>Davide Manuel Alves Da Silva</t>
+  </si>
+  <si>
+    <t>Berri Lantegia</t>
+  </si>
+  <si>
+    <t>24380480  </t>
+  </si>
+  <si>
+    <t>Todo Maq. Agric. Jard., S.L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bricogarden Center la Mancha </t>
+  </si>
+  <si>
+    <t>No liberar NUNCA</t>
+  </si>
+  <si>
+    <t>Bosque y Jardin Algama, S.L.</t>
+  </si>
+  <si>
+    <t>Comercial Serrano Baños, S.L.U </t>
+  </si>
+  <si>
+    <t>José Gil Blazquez, C.B.</t>
+  </si>
+  <si>
+    <t>Alfred Lolo Sampron</t>
+  </si>
+  <si>
+    <t>Pedro Ramón Alpeñes Gamon</t>
+  </si>
+  <si>
+    <t>Integral Maquinaria y Taller,S.L. </t>
+  </si>
+  <si>
+    <t>24022030 </t>
+  </si>
+  <si>
+    <t>Forestal Andión,S.L.</t>
+  </si>
+  <si>
+    <t>Garaje Aurtenetxe, S.A.</t>
+  </si>
+  <si>
+    <t>Suministros Maquival</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,9 +399,22 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF32363A"/>
+      <name val="72"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="72"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +424,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F7F7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -411,7 +475,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
@@ -423,6 +487,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
@@ -772,10 +840,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC2B6E0-CB86-444E-845A-38B69EC4F7CA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -834,7 +902,7 @@
         <v>24291920</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
@@ -843,43 +911,43 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>24040720</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>24080530</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>24440820</v>
+        <v>24040720</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>24330260</v>
+        <v>24440820</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>14</v>
@@ -887,195 +955,195 @@
     </row>
     <row r="8" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>24370920</v>
+        <v>24330260</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>24150930</v>
+        <v>24370920</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>24310810</v>
+        <v>24150930</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>24360040</v>
+        <v>24310810</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>24160920</v>
+        <v>24360040</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>24410190</v>
+        <v>24160920</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>24040650</v>
+        <v>24410190</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
+        <v>24040650</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <v>24356000</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>24100070</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>24062760</v>
+        <v>24100070</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>24320360</v>
+        <v>24062760</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>24460620</v>
+        <v>24320360</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>24160540</v>
+        <v>24460620</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>22</v>
@@ -1083,69 +1151,69 @@
     </row>
     <row r="22" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>24160870</v>
+        <v>24160540</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>24450220</v>
+        <v>24160870</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>24140420</v>
+        <v>24450220</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>24380400</v>
+        <v>24140420</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>24350380</v>
+        <v>24380400</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>46</v>
@@ -1153,27 +1221,27 @@
     </row>
     <row r="27" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>24380330</v>
+        <v>24350380</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>24050950</v>
+        <v>24380330</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>49</v>
@@ -1181,96 +1249,249 @@
     </row>
     <row r="29" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>24410480</v>
+        <v>24050950</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>24292010</v>
+        <v>24410480</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="5">
+        <v>24292010</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>24062820</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>24050540</v>
+        <v>24062820</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>24050540</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
         <v>24380290</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
         <v>24160890</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D36" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>24310750</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="9">
+        <v>24290570</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="9">
+        <v>24380420</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="9">
+        <v>24200180</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="9">
+        <v>24151350</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>24130360</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="9">
+        <v>24151300</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="9">
+        <v>24090590</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>24450160</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1286,7 +1507,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:C3 B4:B35</xm:sqref>
+          <xm:sqref>B2:C3 B4:B47</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1632,26 +1853,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100812FB67C5E01F547A18D4A5FD6A8713D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b9642c6788bad27e02d635fb107c9ae4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xmlns:ns3="d9b07192-7579-4291-b28e-58bbe42d995f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e8472eb4e8570153d151932821fc84c" ns2:_="" ns3:_="">
     <xsd:import namespace="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
@@ -1886,10 +2087,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85648A9D-E349-4AED-A783-3910A6F0B756}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DFC932F-8B19-4888-9E6D-5ED99EBC92C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
+    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1906,20 +2138,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DFC932F-8B19-4888-9E6D-5ED99EBC92C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85648A9D-E349-4AED-A783-3910A6F0B756}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
-    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualizamos versión para descargar correctamente Excel
</commit_message>
<xml_diff>
--- a/Data/TempExcelExport/Clientes con incidencias LC.xlsx
+++ b/Data/TempExcelExport/Clientes con incidencias LC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup.sharepoint.com/sites/IBERICAN_FCI/Shared Documents/1. Clientes/2. Límites de Crédito/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="8_{7AC7CC33-7575-48E7-9E50-6B79B30A2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAC99C16-B388-434A-AF5D-2B375FB0E8E9}"/>
+  <xr:revisionPtr revIDLastSave="388" documentId="8_{7AC7CC33-7575-48E7-9E50-6B79B30A2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{678CC7DB-1BEC-4CD8-A971-A5134243E762}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="13125" windowHeight="11235" firstSheet="1" activeTab="1" xr2:uid="{80C2A359-1417-4DB8-9FCF-050718A4EF94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{80C2A359-1417-4DB8-9FCF-050718A4EF94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" state="veryHidden" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="94">
   <si>
     <t>Cliente</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Ramón García Ocaña / 16400 Tarancón</t>
   </si>
   <si>
-    <t>Liberar mientras no supere "Open invoices"10 mil €</t>
-  </si>
-  <si>
     <t>Repuestos Hnos. Garvi, S.L. / 23360 La Puerta de S</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>Agromecánica Ismael, S.L. / 04710 Santa Mª del Agu</t>
   </si>
   <si>
-    <t>Joaquin Hernandez E Hijos, S.L</t>
-  </si>
-  <si>
     <t>Felijardim de Mario Felicia</t>
   </si>
   <si>
@@ -304,38 +298,35 @@
     <t>Bosque y Jardin Algama, S.L.</t>
   </si>
   <si>
-    <t>Comercial Serrano Baños, S.L.U </t>
-  </si>
-  <si>
     <t>José Gil Blazquez, C.B.</t>
   </si>
   <si>
-    <t>Alfred Lolo Sampron</t>
-  </si>
-  <si>
     <t>Pedro Ramón Alpeñes Gamon</t>
   </si>
   <si>
-    <t>Integral Maquinaria y Taller,S.L. </t>
-  </si>
-  <si>
-    <t>24022030 </t>
-  </si>
-  <si>
-    <t>Forestal Andión,S.L.</t>
-  </si>
-  <si>
-    <t>Garaje Aurtenetxe, S.A.</t>
-  </si>
-  <si>
     <t>Suministros Maquival</t>
+  </si>
+  <si>
+    <t>Juan Cortiada, S.L.</t>
+  </si>
+  <si>
+    <t>NO LIBERAR NADA, sólo si paga por anticipado, concurso acreedores</t>
+  </si>
+  <si>
+    <t>Agroforestal Jaén</t>
+  </si>
+  <si>
+    <t>Comercial Escallada, S.L.</t>
+  </si>
+  <si>
+    <t>Esperar hasta reunión con Ana 26/02/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,20 +392,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF32363A"/>
-      <name val="72"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="72"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,12 +403,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7F7F7"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -475,7 +448,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
@@ -487,10 +460,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
@@ -840,15 +809,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC2B6E0-CB86-444E-845A-38B69EC4F7CA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.25" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="42.25" style="3" customWidth="1"/>
@@ -902,7 +871,7 @@
         <v>24291920</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
@@ -911,18 +880,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>24080530</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -944,7 +913,7 @@
         <v>24440820</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
@@ -1126,13 +1095,10 @@
         <v>24320360</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1143,7 +1109,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>22</v>
@@ -1157,7 +1123,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>22</v>
@@ -1171,7 +1137,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
@@ -1185,10 +1151,10 @@
         <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1199,10 +1165,10 @@
         <v>9</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1213,10 +1179,10 @@
         <v>9</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1227,10 +1193,10 @@
         <v>9</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1241,10 +1207,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1252,13 +1218,13 @@
         <v>24050950</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1269,231 +1235,198 @@
         <v>4</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
-        <v>24292010</v>
+      <c r="A31" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>74</v>
+      <c r="A32" s="5">
+        <v>24062820</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="33" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>24062820</v>
+        <v>24050540</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>24050540</v>
+        <v>24380290</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>24380290</v>
+        <v>24160890</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
         <v>79</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
-        <v>24160890</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>24310750</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
-        <v>24310750</v>
+    </row>
+    <row r="38" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>24290570</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>85</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>24200180</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="9">
-        <v>24290570</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="9" t="s">
+    <row r="40" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>24130360</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="9">
-        <v>24380420</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="9" t="s">
+      <c r="D40" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>24450160</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="9">
-        <v>24200180</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="9" t="s">
+    <row r="42" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>24150090</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="9">
-        <v>24151350</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="10" t="s">
+      <c r="D42" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="9">
-        <v>24130360</v>
+    <row r="43" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>24460650</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="3" t="s">
         <v>91</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="9">
-        <v>24151300</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>24062600</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="9">
-        <v>24090590</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
-        <v>24450160</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>80</v>
-      </c>
+    <row r="45" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1507,7 +1440,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:C3 B4:B47</xm:sqref>
+          <xm:sqref>B2:C3 B4:B44</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1554,10 +1487,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1568,10 +1501,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1582,10 +1515,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1596,10 +1529,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1610,10 +1543,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1624,10 +1557,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1638,10 +1571,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1652,10 +1585,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1666,10 +1599,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1680,10 +1613,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1694,10 +1627,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1708,10 +1641,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1722,24 +1655,24 @@
         <v>4</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
v1.0.56 - Cambiado pickbranch cierre Excel a Switch
</commit_message>
<xml_diff>
--- a/Data/TempExcelExport/Clientes con incidencias LC.xlsx
+++ b/Data/TempExcelExport/Clientes con incidencias LC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup.sharepoint.com/sites/IBERICAN_FCI/Shared Documents/1. Clientes/2. Límites de Crédito/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="388" documentId="8_{7AC7CC33-7575-48E7-9E50-6B79B30A2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{678CC7DB-1BEC-4CD8-A971-A5134243E762}"/>
+  <xr:revisionPtr revIDLastSave="450" documentId="8_{7AC7CC33-7575-48E7-9E50-6B79B30A2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D7C837C-A22F-4119-A431-2A5C45179E8D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{80C2A359-1417-4DB8-9FCF-050718A4EF94}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="14340" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{80C2A359-1417-4DB8-9FCF-050718A4EF94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" state="veryHidden" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
   <si>
     <t>Cliente</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Angel Roldán García / 28033 Madrid</t>
   </si>
   <si>
-    <t>Liberar con precaución de no sobrepasar su LC, tiene aplazamiento y no ha contestado a la proforma.</t>
-  </si>
-  <si>
     <t>Crespo Maquinaria, S.L. / 36820 Pte Caldelas</t>
   </si>
   <si>
@@ -256,15 +253,6 @@
     <t>Live Our Style</t>
   </si>
   <si>
-    <t>24050970  </t>
-  </si>
-  <si>
-    <t>Antonio Fernandez Del Riego</t>
-  </si>
-  <si>
-    <t>NO LIBERAR NADA,VZ7 solicita precaución</t>
-  </si>
-  <si>
     <t>Alba Fernandez Fernandez / 39691 Iruz</t>
   </si>
   <si>
@@ -320,13 +308,40 @@
   </si>
   <si>
     <t>Esperar hasta reunión con Ana 26/02/2025</t>
+  </si>
+  <si>
+    <t>24340420  </t>
+  </si>
+  <si>
+    <t>Grupo Nombela,S.L</t>
+  </si>
+  <si>
+    <t>Maq.de Jardinería Rial,S.L.U </t>
+  </si>
+  <si>
+    <t>No liberar por encima de su LC.Pide mucho y luego tiene problemas de liquidez</t>
+  </si>
+  <si>
+    <t>No liberar tiene impagado con Aplazamiento</t>
+  </si>
+  <si>
+    <t>Marcelo Alejandro Moreno</t>
+  </si>
+  <si>
+    <t>Forestal Andión</t>
+  </si>
+  <si>
+    <t>Antonio Marin Quintana</t>
+  </si>
+  <si>
+    <t>Bloqueo a Antonio Marín porque ha impagado su hno. Pedro Marín Quintana 24460920</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,8 +407,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF32363A"/>
+      <name val="72"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="72"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +430,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F7F7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -448,18 +481,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
@@ -783,17 +825,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -809,23 +851,23 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC2B6E0-CB86-444E-845A-38B69EC4F7CA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.58203125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.25" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.25" style="10" customWidth="1"/>
     <col min="2" max="2" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="42.25" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.625" style="3"/>
+    <col min="5" max="16384" width="8.58203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -838,8 +880,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="2" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9">
         <v>24370950</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -852,8 +894,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="3" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9">
         <v>24460900</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -866,8 +908,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9">
         <v>24291920</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -877,556 +919,600 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
+        <v>24080530</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9">
+        <v>24040720</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>24080530</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>24040720</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9">
         <v>24440820</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>24330260</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>24330260</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>24370920</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>24370920</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>24150930</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>24150930</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>24310810</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>24310810</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
         <v>24360040</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>24160920</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>24160920</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>24410190</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>24410190</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>24040650</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>24040650</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>24356000</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>24356000</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="3" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="3" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="9">
+        <v>24100070</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>24100070</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="9">
+        <v>24062760</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>24062760</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="3" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9">
+        <v>24320360</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>24320360</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="3" t="s">
+    <row r="21" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9">
+        <v>24460620</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>24460620</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="9">
+        <v>24160540</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>24160540</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="9">
+        <v>24160870</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>24160870</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+    <row r="24" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9">
         <v>24450220</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="3" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="9">
+        <v>24140420</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>24140420</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="3" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="9">
+        <v>24380400</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <v>24380400</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="3" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="9">
+        <v>24350380</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>24350380</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="9">
+        <v>24380330</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>24380330</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="3" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9">
+        <v>24050950</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>24050950</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="9">
+        <v>24410480</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>24410480</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="9">
+        <v>24062820</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9">
+        <v>24050540</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="D32" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9">
+        <v>24380290</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>24062820</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="3" t="s">
+    <row r="34" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="9">
+        <v>24160890</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>24050540</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>24380290</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="B35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>24160890</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="3" t="s">
+    <row r="36" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="9">
+        <v>24310750</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="D36" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="9">
+        <v>24290570</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="D37" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="9">
+        <v>24200180</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>24310750</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="3" t="s">
+    </row>
+    <row r="39" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="9">
+        <v>24130360</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="3" t="s">
+    </row>
+    <row r="40" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="9">
+        <v>24450160</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
-        <v>24290570</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="3" t="s">
+    <row r="41" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="9">
+        <v>24150090</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>24200180</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>24130360</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="3" t="s">
+    <row r="42" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="9">
+        <v>24460650</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>24450160</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="D42" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="9">
+        <v>24062600</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>24150090</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="3" t="s">
+    <row r="44" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
-        <v>24460650</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="B44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="9">
+        <v>24011760</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
-        <v>24062600</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
+    <row r="46" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="9">
+        <v>24470930</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="9">
+        <v>24022030</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="10">
+        <v>24460820</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1440,7 +1526,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:C3 B4:B44</xm:sqref>
+          <xm:sqref>B2:C3 B4:B48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1457,15 +1543,15 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.625" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1479,291 +1565,291 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+    <row r="2" spans="1:4" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>46710570</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>46730050</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>46730050</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>46680120</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>46680120</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="6" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>46700030</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>46700030</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>46730280</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>46730280</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>46750090</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>46750090</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>46730070</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>46730070</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>46730250</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>46730250</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="6" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>46730290</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>46730290</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>46680190</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>46680190</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>46730180</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>46730180</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>46710600</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>46710600</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>46750050</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>46750050</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="D15" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1786,6 +1872,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100812FB67C5E01F547A18D4A5FD6A8713D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b9642c6788bad27e02d635fb107c9ae4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xmlns:ns3="d9b07192-7579-4291-b28e-58bbe42d995f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e8472eb4e8570153d151932821fc84c" ns2:_="" ns3:_="">
     <xsd:import namespace="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
@@ -2020,7 +2115,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
@@ -2031,16 +2126,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85648A9D-E349-4AED-A783-3910A6F0B756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DFC932F-8B19-4888-9E6D-5ED99EBC92C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2059,7 +2153,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498E4CA6-DBB7-44FA-89D6-924D2B3C9ABD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2068,12 +2162,4 @@
     <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85648A9D-E349-4AED-A783-3910A6F0B756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>